<commit_message>
removed financial stuff; new price table; discount
</commit_message>
<xml_diff>
--- a/generator/masterdata.xlsx
+++ b/generator/masterdata.xlsx
@@ -3,15 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A102F3D3-58E9-473F-A04D-0DA0FEC1067A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F0DFD6C-DE74-4E19-8C23-FF9C12738E41}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="10500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="10500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="years" sheetId="4" r:id="rId1"/>
+    <sheet name="years" sheetId="7" r:id="rId1"/>
     <sheet name="weeks" sheetId="3" r:id="rId2"/>
     <sheet name="customers" sheetId="1" r:id="rId3"/>
     <sheet name="materials" sheetId="2" r:id="rId4"/>
+    <sheet name="prices EUR" sheetId="5" r:id="rId5"/>
+    <sheet name="prices USD" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -23,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="129">
   <si>
     <t>Rocky Mountain Bikes</t>
   </si>
@@ -304,115 +306,112 @@
     <t>Reason</t>
   </si>
   <si>
+    <t>VKORG</t>
+  </si>
+  <si>
+    <t>VTWEG</t>
+  </si>
+  <si>
+    <t>SPART</t>
+  </si>
+  <si>
+    <t>BI</t>
+  </si>
+  <si>
+    <t>WH</t>
+  </si>
+  <si>
+    <t>DS00</t>
+  </si>
+  <si>
+    <t>DN00</t>
+  </si>
+  <si>
+    <t>UE00</t>
+  </si>
+  <si>
+    <t>UW00</t>
+  </si>
+  <si>
+    <t>RHMT1000</t>
+  </si>
+  <si>
+    <t>RKIT1000</t>
+  </si>
+  <si>
+    <t>SHRT1000</t>
+  </si>
+  <si>
+    <t>BOTL1000</t>
+  </si>
+  <si>
+    <t>CAGE1000</t>
+  </si>
+  <si>
+    <t>DGRB2000</t>
+  </si>
+  <si>
+    <t>DGRR2000</t>
+  </si>
+  <si>
+    <t>DGRW2000</t>
+  </si>
+  <si>
+    <t>DXTR1000</t>
+  </si>
+  <si>
+    <t>DXTR2000</t>
+  </si>
+  <si>
+    <t>DXTR3000</t>
+  </si>
+  <si>
+    <t>EPAD1000</t>
+  </si>
+  <si>
+    <t>FAID1000</t>
+  </si>
+  <si>
+    <t>GRBL2000</t>
+  </si>
+  <si>
+    <t>GRRL2000</t>
+  </si>
+  <si>
+    <t>GRWL2000</t>
+  </si>
+  <si>
+    <t>KPAD1000</t>
+  </si>
+  <si>
+    <t>OHMT1000</t>
+  </si>
+  <si>
+    <t>ORBC1000</t>
+  </si>
+  <si>
+    <t>ORMN1000</t>
+  </si>
+  <si>
+    <t>ORWN1000</t>
+  </si>
+  <si>
+    <t>PRTR1000</t>
+  </si>
+  <si>
+    <t>PRTR2000</t>
+  </si>
+  <si>
+    <t>PRTR3000</t>
+  </si>
+  <si>
+    <t>PUMP1000</t>
+  </si>
+  <si>
     <t>Year</t>
   </si>
   <si>
     <t>Growth</t>
-  </si>
-  <si>
-    <t>Salesprice</t>
-  </si>
-  <si>
-    <t>VKORG</t>
-  </si>
-  <si>
-    <t>VTWEG</t>
-  </si>
-  <si>
-    <t>SPART</t>
-  </si>
-  <si>
-    <t>BI</t>
-  </si>
-  <si>
-    <t>WH</t>
-  </si>
-  <si>
-    <t>DS00</t>
-  </si>
-  <si>
-    <t>DN00</t>
-  </si>
-  <si>
-    <t>UE00</t>
-  </si>
-  <si>
-    <t>UW00</t>
-  </si>
-  <si>
-    <t>RHMT1000</t>
-  </si>
-  <si>
-    <t>RKIT1000</t>
-  </si>
-  <si>
-    <t>SHRT1000</t>
-  </si>
-  <si>
-    <t>BOTL1000</t>
-  </si>
-  <si>
-    <t>CAGE1000</t>
-  </si>
-  <si>
-    <t>DGRB2000</t>
-  </si>
-  <si>
-    <t>DGRR2000</t>
-  </si>
-  <si>
-    <t>DGRW2000</t>
-  </si>
-  <si>
-    <t>DXTR1000</t>
-  </si>
-  <si>
-    <t>DXTR2000</t>
-  </si>
-  <si>
-    <t>DXTR3000</t>
-  </si>
-  <si>
-    <t>EPAD1000</t>
-  </si>
-  <si>
-    <t>FAID1000</t>
-  </si>
-  <si>
-    <t>GRBL2000</t>
-  </si>
-  <si>
-    <t>GRRL2000</t>
-  </si>
-  <si>
-    <t>GRWL2000</t>
-  </si>
-  <si>
-    <t>KPAD1000</t>
-  </si>
-  <si>
-    <t>OHMT1000</t>
-  </si>
-  <si>
-    <t>ORBC1000</t>
-  </si>
-  <si>
-    <t>ORMN1000</t>
-  </si>
-  <si>
-    <t>ORWN1000</t>
-  </si>
-  <si>
-    <t>PRTR1000</t>
-  </si>
-  <si>
-    <t>PRTR2000</t>
-  </si>
-  <si>
-    <t>PRTR3000</t>
-  </si>
-  <si>
-    <t>PUMP1000</t>
   </si>
 </sst>
 </file>
@@ -756,10 +755,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F085220-F61A-4D10-9AB9-F0D53D15F226}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23D9E596-51CC-440C-8BFE-8B4B0D6F8F00}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -767,10 +766,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>93</v>
+        <v>127</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>94</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1362,7 +1361,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1387,13 +1386,13 @@
         <v>87</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -1410,13 +1409,13 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -1433,13 +1432,13 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -1456,13 +1455,13 @@
         <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -1479,13 +1478,13 @@
         <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1502,13 +1501,13 @@
         <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1525,13 +1524,13 @@
         <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -1548,13 +1547,13 @@
         <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G8" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -1571,13 +1570,13 @@
         <v>10</v>
       </c>
       <c r="E9" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G9" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -1594,13 +1593,13 @@
         <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G10" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -1617,13 +1616,13 @@
         <v>8</v>
       </c>
       <c r="E11" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G11" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -1640,13 +1639,13 @@
         <v>5</v>
       </c>
       <c r="E12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G12" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -1663,13 +1662,13 @@
         <v>10</v>
       </c>
       <c r="E13" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G13" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -1686,13 +1685,13 @@
         <v>10</v>
       </c>
       <c r="E14" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G14" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -1709,13 +1708,13 @@
         <v>10</v>
       </c>
       <c r="E15" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G15" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -1732,13 +1731,13 @@
         <v>5</v>
       </c>
       <c r="E16" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G16" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -1755,13 +1754,13 @@
         <v>10</v>
       </c>
       <c r="E17" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G17" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -1778,13 +1777,13 @@
         <v>10</v>
       </c>
       <c r="E18" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G18" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -1801,13 +1800,13 @@
         <v>15</v>
       </c>
       <c r="E19" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G19" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -1824,13 +1823,13 @@
         <v>12</v>
       </c>
       <c r="E20" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -1847,13 +1846,13 @@
         <v>10</v>
       </c>
       <c r="E21" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G21" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -1867,16 +1866,16 @@
         <v>46</v>
       </c>
       <c r="D22" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G22" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -1893,13 +1892,13 @@
         <v>10</v>
       </c>
       <c r="E23" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G23" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -1916,13 +1915,13 @@
         <v>7</v>
       </c>
       <c r="E24" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G24" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -1939,13 +1938,13 @@
         <v>10</v>
       </c>
       <c r="E25" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G25" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1959,10 +1958,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC2E5201-7E8F-412B-9CA7-DAC430378AA1}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1973,7 +1972,7 @@
     <col min="4" max="4" width="37.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>50</v>
       </c>
@@ -1989,13 +1988,10 @@
       <c r="E1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s">
         <v>54</v>
@@ -2009,466 +2005,3362 @@
       <c r="E2">
         <v>1</v>
       </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>110</v>
+      </c>
+      <c r="B7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>113</v>
+      </c>
+      <c r="B10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E10">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" t="s">
+        <v>68</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>115</v>
+      </c>
+      <c r="B12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>116</v>
+      </c>
+      <c r="B13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" t="s">
+        <v>70</v>
+      </c>
+      <c r="E13">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>117</v>
+      </c>
+      <c r="B14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>118</v>
+      </c>
+      <c r="B15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" t="s">
+        <v>72</v>
+      </c>
+      <c r="E15">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>119</v>
+      </c>
+      <c r="B16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>120</v>
+      </c>
+      <c r="B17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" t="s">
+        <v>74</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>121</v>
+      </c>
+      <c r="B18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" t="s">
+        <v>75</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>122</v>
+      </c>
+      <c r="B19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" t="s">
+        <v>76</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>123</v>
+      </c>
+      <c r="B20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" t="s">
+        <v>77</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>124</v>
+      </c>
+      <c r="B21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" t="s">
+        <v>78</v>
+      </c>
+      <c r="E21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>125</v>
+      </c>
+      <c r="B22" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" t="s">
+        <v>79</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>126</v>
+      </c>
+      <c r="B23" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" t="s">
+        <v>80</v>
+      </c>
+      <c r="E23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>102</v>
+      </c>
+      <c r="B24" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24" t="s">
+        <v>81</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>103</v>
+      </c>
+      <c r="B25" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25" t="s">
+        <v>82</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>104</v>
+      </c>
+      <c r="B26" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" t="s">
+        <v>83</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD0D86CA-C480-4207-978B-DFF5473555A0}">
+  <dimension ref="A1:R26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="18" width="7.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2023</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2024</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2025</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2026</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2027</v>
+      </c>
+      <c r="K1" s="1">
+        <v>2028</v>
+      </c>
+      <c r="L1" s="1">
+        <v>2029</v>
+      </c>
+      <c r="M1" s="1">
+        <v>2030</v>
+      </c>
+      <c r="N1" s="1">
+        <v>2031</v>
+      </c>
+      <c r="O1" s="1">
+        <v>2032</v>
+      </c>
+      <c r="P1" s="1">
+        <v>2033</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>2034</v>
+      </c>
+      <c r="R1" s="1">
+        <v>2035</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2">
+        <v>20</v>
+      </c>
+      <c r="D2">
+        <v>20</v>
+      </c>
+      <c r="E2">
+        <v>20</v>
+      </c>
       <c r="F2">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2">
+        <v>20</v>
+      </c>
+      <c r="H2">
+        <v>20</v>
+      </c>
+      <c r="I2">
+        <v>20</v>
+      </c>
+      <c r="J2">
+        <v>20</v>
+      </c>
+      <c r="K2">
+        <v>20</v>
+      </c>
+      <c r="L2">
+        <v>20</v>
+      </c>
+      <c r="M2">
+        <v>20</v>
+      </c>
+      <c r="N2">
+        <v>20</v>
+      </c>
+      <c r="O2">
+        <v>20</v>
+      </c>
+      <c r="P2">
+        <v>20</v>
+      </c>
+      <c r="Q2">
+        <v>20</v>
+      </c>
+      <c r="R2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D3" t="s">
         <v>57</v>
       </c>
+      <c r="C3">
+        <v>18</v>
+      </c>
+      <c r="D3">
+        <v>18</v>
+      </c>
       <c r="E3">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="F3">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3">
+        <v>18</v>
+      </c>
+      <c r="H3">
+        <v>18</v>
+      </c>
+      <c r="I3">
+        <v>18</v>
+      </c>
+      <c r="J3">
+        <v>18</v>
+      </c>
+      <c r="K3">
+        <v>18</v>
+      </c>
+      <c r="L3">
+        <v>18</v>
+      </c>
+      <c r="M3">
+        <v>18</v>
+      </c>
+      <c r="N3">
+        <v>18</v>
+      </c>
+      <c r="O3">
+        <v>18</v>
+      </c>
+      <c r="P3">
+        <v>18</v>
+      </c>
+      <c r="Q3">
+        <v>18</v>
+      </c>
+      <c r="R3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4">
+        <v>390</v>
+      </c>
+      <c r="D4">
+        <v>390</v>
+      </c>
+      <c r="E4">
+        <v>390</v>
+      </c>
+      <c r="F4">
+        <v>390</v>
+      </c>
+      <c r="G4">
+        <v>390</v>
+      </c>
+      <c r="H4">
+        <v>390</v>
+      </c>
+      <c r="I4">
+        <v>390</v>
+      </c>
+      <c r="J4">
+        <v>390</v>
+      </c>
+      <c r="K4">
+        <v>390</v>
+      </c>
+      <c r="L4">
+        <v>390</v>
+      </c>
+      <c r="M4">
+        <v>390</v>
+      </c>
+      <c r="N4">
+        <v>390</v>
+      </c>
+      <c r="O4">
+        <v>390</v>
+      </c>
+      <c r="P4">
+        <v>390</v>
+      </c>
+      <c r="Q4">
+        <v>390</v>
+      </c>
+      <c r="R4">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5">
+        <v>390</v>
+      </c>
+      <c r="D5">
+        <v>390</v>
+      </c>
+      <c r="E5">
+        <v>390</v>
+      </c>
+      <c r="F5">
+        <v>390</v>
+      </c>
+      <c r="G5">
+        <v>390</v>
+      </c>
+      <c r="H5">
+        <v>390</v>
+      </c>
+      <c r="I5">
+        <v>390</v>
+      </c>
+      <c r="J5">
+        <v>390</v>
+      </c>
+      <c r="K5">
+        <v>390</v>
+      </c>
+      <c r="L5">
+        <v>390</v>
+      </c>
+      <c r="M5">
+        <v>390</v>
+      </c>
+      <c r="N5">
+        <v>390</v>
+      </c>
+      <c r="O5">
+        <v>390</v>
+      </c>
+      <c r="P5">
+        <v>390</v>
+      </c>
+      <c r="Q5">
+        <v>390</v>
+      </c>
+      <c r="R5">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6">
+        <v>390</v>
+      </c>
+      <c r="D6">
+        <v>390</v>
+      </c>
+      <c r="E6">
+        <v>390</v>
+      </c>
+      <c r="F6">
+        <v>390</v>
+      </c>
+      <c r="G6">
+        <v>390</v>
+      </c>
+      <c r="H6">
+        <v>390</v>
+      </c>
+      <c r="I6">
+        <v>390</v>
+      </c>
+      <c r="J6">
+        <v>390</v>
+      </c>
+      <c r="K6">
+        <v>390</v>
+      </c>
+      <c r="L6">
+        <v>390</v>
+      </c>
+      <c r="M6">
+        <v>390</v>
+      </c>
+      <c r="N6">
+        <v>390</v>
+      </c>
+      <c r="O6">
+        <v>390</v>
+      </c>
+      <c r="P6">
+        <v>390</v>
+      </c>
+      <c r="Q6">
+        <v>390</v>
+      </c>
+      <c r="R6">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>110</v>
       </c>
-      <c r="B4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E4">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="B7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7">
+        <v>3000</v>
+      </c>
+      <c r="D7">
+        <v>3000</v>
+      </c>
+      <c r="E7">
+        <v>3000</v>
+      </c>
+      <c r="F7">
+        <v>3000</v>
+      </c>
+      <c r="G7">
+        <v>3000</v>
+      </c>
+      <c r="H7">
+        <v>3000</v>
+      </c>
+      <c r="I7">
+        <v>3000</v>
+      </c>
+      <c r="J7">
+        <v>3000</v>
+      </c>
+      <c r="K7">
+        <v>3000</v>
+      </c>
+      <c r="L7">
+        <v>3000</v>
+      </c>
+      <c r="M7">
+        <v>3000</v>
+      </c>
+      <c r="N7">
+        <v>3000</v>
+      </c>
+      <c r="O7">
+        <v>3000</v>
+      </c>
+      <c r="P7">
+        <v>3000</v>
+      </c>
+      <c r="Q7">
+        <v>3000</v>
+      </c>
+      <c r="R7">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>111</v>
       </c>
-      <c r="B5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E5">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="B8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8">
+        <v>3000</v>
+      </c>
+      <c r="D8">
+        <v>3000</v>
+      </c>
+      <c r="E8">
+        <v>3000</v>
+      </c>
+      <c r="F8">
+        <v>3000</v>
+      </c>
+      <c r="G8">
+        <v>3000</v>
+      </c>
+      <c r="H8">
+        <v>3000</v>
+      </c>
+      <c r="I8">
+        <v>3000</v>
+      </c>
+      <c r="J8">
+        <v>3000</v>
+      </c>
+      <c r="K8">
+        <v>3000</v>
+      </c>
+      <c r="L8">
+        <v>3000</v>
+      </c>
+      <c r="M8">
+        <v>3000</v>
+      </c>
+      <c r="N8">
+        <v>3000</v>
+      </c>
+      <c r="O8">
+        <v>3000</v>
+      </c>
+      <c r="P8">
+        <v>3000</v>
+      </c>
+      <c r="Q8">
+        <v>3000</v>
+      </c>
+      <c r="R8">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>112</v>
       </c>
-      <c r="B6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D6" t="s">
-        <v>61</v>
-      </c>
-      <c r="E6">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="B9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9">
+        <v>3000</v>
+      </c>
+      <c r="D9">
+        <v>3000</v>
+      </c>
+      <c r="E9">
+        <v>3000</v>
+      </c>
+      <c r="F9">
+        <v>3000</v>
+      </c>
+      <c r="G9">
+        <v>3000</v>
+      </c>
+      <c r="H9">
+        <v>3000</v>
+      </c>
+      <c r="I9">
+        <v>3000</v>
+      </c>
+      <c r="J9">
+        <v>3000</v>
+      </c>
+      <c r="K9">
+        <v>3000</v>
+      </c>
+      <c r="L9">
+        <v>3000</v>
+      </c>
+      <c r="M9">
+        <v>3000</v>
+      </c>
+      <c r="N9">
+        <v>3000</v>
+      </c>
+      <c r="O9">
+        <v>3000</v>
+      </c>
+      <c r="P9">
+        <v>3000</v>
+      </c>
+      <c r="Q9">
+        <v>3000</v>
+      </c>
+      <c r="R9">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>113</v>
       </c>
-      <c r="B7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D7" t="s">
-        <v>63</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="B10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10">
+        <v>75</v>
+      </c>
+      <c r="D10">
+        <v>75</v>
+      </c>
+      <c r="E10">
+        <v>75</v>
+      </c>
+      <c r="F10">
+        <v>75</v>
+      </c>
+      <c r="G10">
+        <v>75</v>
+      </c>
+      <c r="H10">
+        <v>75</v>
+      </c>
+      <c r="I10">
+        <v>75</v>
+      </c>
+      <c r="J10">
+        <v>75</v>
+      </c>
+      <c r="K10">
+        <v>75</v>
+      </c>
+      <c r="L10">
+        <v>75</v>
+      </c>
+      <c r="M10">
+        <v>75</v>
+      </c>
+      <c r="N10">
+        <v>75</v>
+      </c>
+      <c r="O10">
+        <v>75</v>
+      </c>
+      <c r="P10">
+        <v>75</v>
+      </c>
+      <c r="Q10">
+        <v>75</v>
+      </c>
+      <c r="R10">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>114</v>
       </c>
-      <c r="B8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D8" t="s">
-        <v>64</v>
-      </c>
-      <c r="E8">
-        <v>2</v>
-      </c>
-      <c r="F8">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>115</v>
-      </c>
-      <c r="B9" t="s">
-        <v>62</v>
-      </c>
-      <c r="C9" t="s">
-        <v>58</v>
-      </c>
-      <c r="D9" t="s">
-        <v>65</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>116</v>
-      </c>
-      <c r="B10" t="s">
-        <v>66</v>
-      </c>
-      <c r="C10" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" t="s">
-        <v>67</v>
-      </c>
-      <c r="E10">
-        <v>0.5</v>
-      </c>
-      <c r="F10">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>117</v>
-      </c>
       <c r="B11" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D11" t="s">
         <v>68</v>
       </c>
+      <c r="C11">
+        <v>40</v>
+      </c>
+      <c r="D11">
+        <v>40</v>
+      </c>
       <c r="E11">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="F11">
         <v>40</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G11">
+        <v>40</v>
+      </c>
+      <c r="H11">
+        <v>40</v>
+      </c>
+      <c r="I11">
+        <v>40</v>
+      </c>
+      <c r="J11">
+        <v>40</v>
+      </c>
+      <c r="K11">
+        <v>40</v>
+      </c>
+      <c r="L11">
+        <v>40</v>
+      </c>
+      <c r="M11">
+        <v>40</v>
+      </c>
+      <c r="N11">
+        <v>40</v>
+      </c>
+      <c r="O11">
+        <v>40</v>
+      </c>
+      <c r="P11">
+        <v>40</v>
+      </c>
+      <c r="Q11">
+        <v>40</v>
+      </c>
+      <c r="R11">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>115</v>
+      </c>
+      <c r="B12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12">
+        <v>330</v>
+      </c>
+      <c r="D12">
+        <v>330</v>
+      </c>
+      <c r="E12">
+        <v>330</v>
+      </c>
+      <c r="F12">
+        <v>330</v>
+      </c>
+      <c r="G12">
+        <v>330</v>
+      </c>
+      <c r="H12">
+        <v>330</v>
+      </c>
+      <c r="I12">
+        <v>330</v>
+      </c>
+      <c r="J12">
+        <v>330</v>
+      </c>
+      <c r="K12">
+        <v>330</v>
+      </c>
+      <c r="L12">
+        <v>330</v>
+      </c>
+      <c r="M12">
+        <v>330</v>
+      </c>
+      <c r="N12">
+        <v>330</v>
+      </c>
+      <c r="O12">
+        <v>330</v>
+      </c>
+      <c r="P12">
+        <v>330</v>
+      </c>
+      <c r="Q12">
+        <v>330</v>
+      </c>
+      <c r="R12">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>116</v>
+      </c>
+      <c r="B13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13">
+        <v>330</v>
+      </c>
+      <c r="D13">
+        <v>330</v>
+      </c>
+      <c r="E13">
+        <v>330</v>
+      </c>
+      <c r="F13">
+        <v>330</v>
+      </c>
+      <c r="G13">
+        <v>330</v>
+      </c>
+      <c r="H13">
+        <v>330</v>
+      </c>
+      <c r="I13">
+        <v>330</v>
+      </c>
+      <c r="J13">
+        <v>330</v>
+      </c>
+      <c r="K13">
+        <v>330</v>
+      </c>
+      <c r="L13">
+        <v>330</v>
+      </c>
+      <c r="M13">
+        <v>330</v>
+      </c>
+      <c r="N13">
+        <v>330</v>
+      </c>
+      <c r="O13">
+        <v>330</v>
+      </c>
+      <c r="P13">
+        <v>330</v>
+      </c>
+      <c r="Q13">
+        <v>330</v>
+      </c>
+      <c r="R13">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>117</v>
+      </c>
+      <c r="B14" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14">
+        <v>330</v>
+      </c>
+      <c r="D14">
+        <v>330</v>
+      </c>
+      <c r="E14">
+        <v>330</v>
+      </c>
+      <c r="F14">
+        <v>330</v>
+      </c>
+      <c r="G14">
+        <v>330</v>
+      </c>
+      <c r="H14">
+        <v>330</v>
+      </c>
+      <c r="I14">
+        <v>330</v>
+      </c>
+      <c r="J14">
+        <v>330</v>
+      </c>
+      <c r="K14">
+        <v>330</v>
+      </c>
+      <c r="L14">
+        <v>330</v>
+      </c>
+      <c r="M14">
+        <v>330</v>
+      </c>
+      <c r="N14">
+        <v>330</v>
+      </c>
+      <c r="O14">
+        <v>330</v>
+      </c>
+      <c r="P14">
+        <v>330</v>
+      </c>
+      <c r="Q14">
+        <v>330</v>
+      </c>
+      <c r="R14">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>118</v>
       </c>
-      <c r="B12" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" t="s">
-        <v>58</v>
-      </c>
-      <c r="D12" t="s">
-        <v>69</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="B15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15">
+        <v>75</v>
+      </c>
+      <c r="D15">
+        <v>75</v>
+      </c>
+      <c r="E15">
+        <v>75</v>
+      </c>
+      <c r="F15">
+        <v>75</v>
+      </c>
+      <c r="G15">
+        <v>75</v>
+      </c>
+      <c r="H15">
+        <v>75</v>
+      </c>
+      <c r="I15">
+        <v>75</v>
+      </c>
+      <c r="J15">
+        <v>75</v>
+      </c>
+      <c r="K15">
+        <v>75</v>
+      </c>
+      <c r="L15">
+        <v>75</v>
+      </c>
+      <c r="M15">
+        <v>75</v>
+      </c>
+      <c r="N15">
+        <v>75</v>
+      </c>
+      <c r="O15">
+        <v>75</v>
+      </c>
+      <c r="P15">
+        <v>75</v>
+      </c>
+      <c r="Q15">
+        <v>75</v>
+      </c>
+      <c r="R15">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>119</v>
       </c>
-      <c r="B13" t="s">
-        <v>54</v>
-      </c>
-      <c r="C13" t="s">
-        <v>58</v>
-      </c>
-      <c r="D13" t="s">
-        <v>70</v>
-      </c>
-      <c r="E13">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="B16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16">
+        <v>50</v>
+      </c>
+      <c r="D16">
+        <v>50</v>
+      </c>
+      <c r="E16">
+        <v>50</v>
+      </c>
+      <c r="F16">
+        <v>50</v>
+      </c>
+      <c r="G16">
+        <v>50</v>
+      </c>
+      <c r="H16">
+        <v>50</v>
+      </c>
+      <c r="I16">
+        <v>50</v>
+      </c>
+      <c r="J16">
+        <v>50</v>
+      </c>
+      <c r="K16">
+        <v>50</v>
+      </c>
+      <c r="L16">
+        <v>50</v>
+      </c>
+      <c r="M16">
+        <v>50</v>
+      </c>
+      <c r="N16">
+        <v>50</v>
+      </c>
+      <c r="O16">
+        <v>50</v>
+      </c>
+      <c r="P16">
+        <v>50</v>
+      </c>
+      <c r="Q16">
+        <v>50</v>
+      </c>
+      <c r="R16">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>120</v>
       </c>
-      <c r="B14" t="s">
-        <v>54</v>
-      </c>
-      <c r="C14" t="s">
-        <v>58</v>
-      </c>
-      <c r="D14" t="s">
-        <v>71</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="B17" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17">
+        <v>250</v>
+      </c>
+      <c r="D17">
+        <v>250</v>
+      </c>
+      <c r="E17">
+        <v>250</v>
+      </c>
+      <c r="F17">
+        <v>250</v>
+      </c>
+      <c r="G17">
+        <v>250</v>
+      </c>
+      <c r="H17">
+        <v>250</v>
+      </c>
+      <c r="I17">
+        <v>250</v>
+      </c>
+      <c r="J17">
+        <v>250</v>
+      </c>
+      <c r="K17">
+        <v>250</v>
+      </c>
+      <c r="L17">
+        <v>250</v>
+      </c>
+      <c r="M17">
+        <v>250</v>
+      </c>
+      <c r="N17">
+        <v>250</v>
+      </c>
+      <c r="O17">
+        <v>250</v>
+      </c>
+      <c r="P17">
+        <v>250</v>
+      </c>
+      <c r="Q17">
+        <v>250</v>
+      </c>
+      <c r="R17">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>121</v>
       </c>
-      <c r="B15" t="s">
-        <v>66</v>
-      </c>
-      <c r="C15" t="s">
-        <v>55</v>
-      </c>
-      <c r="D15" t="s">
-        <v>72</v>
-      </c>
-      <c r="E15">
-        <v>0.5</v>
-      </c>
-      <c r="F15">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>122</v>
-      </c>
-      <c r="B16" t="s">
-        <v>66</v>
-      </c>
-      <c r="C16" t="s">
-        <v>55</v>
-      </c>
-      <c r="D16" t="s">
-        <v>73</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="F16">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>123</v>
-      </c>
-      <c r="B17" t="s">
-        <v>54</v>
-      </c>
-      <c r="C17" t="s">
-        <v>58</v>
-      </c>
-      <c r="D17" t="s">
-        <v>74</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>124</v>
-      </c>
       <c r="B18" t="s">
-        <v>62</v>
-      </c>
-      <c r="C18" t="s">
-        <v>58</v>
-      </c>
-      <c r="D18" t="s">
-        <v>75</v>
+        <v>75</v>
+      </c>
+      <c r="C18">
+        <v>2400</v>
+      </c>
+      <c r="D18">
+        <v>2400</v>
       </c>
       <c r="E18">
-        <v>2</v>
+        <v>2400</v>
       </c>
       <c r="F18">
         <v>2400</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G18">
+        <v>2400</v>
+      </c>
+      <c r="H18">
+        <v>2400</v>
+      </c>
+      <c r="I18">
+        <v>2400</v>
+      </c>
+      <c r="J18">
+        <v>2400</v>
+      </c>
+      <c r="K18">
+        <v>2400</v>
+      </c>
+      <c r="L18">
+        <v>2400</v>
+      </c>
+      <c r="M18">
+        <v>2400</v>
+      </c>
+      <c r="N18">
+        <v>2400</v>
+      </c>
+      <c r="O18">
+        <v>2400</v>
+      </c>
+      <c r="P18">
+        <v>2400</v>
+      </c>
+      <c r="Q18">
+        <v>2400</v>
+      </c>
+      <c r="R18">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B19" t="s">
-        <v>62</v>
-      </c>
-      <c r="C19" t="s">
-        <v>58</v>
-      </c>
-      <c r="D19" t="s">
         <v>76</v>
       </c>
+      <c r="C19">
+        <v>2500</v>
+      </c>
+      <c r="D19">
+        <v>2500</v>
+      </c>
       <c r="E19">
-        <v>1</v>
+        <v>2500</v>
       </c>
       <c r="F19">
         <v>2500</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G19">
+        <v>2500</v>
+      </c>
+      <c r="H19">
+        <v>2500</v>
+      </c>
+      <c r="I19">
+        <v>2500</v>
+      </c>
+      <c r="J19">
+        <v>2500</v>
+      </c>
+      <c r="K19">
+        <v>2500</v>
+      </c>
+      <c r="L19">
+        <v>2500</v>
+      </c>
+      <c r="M19">
+        <v>2500</v>
+      </c>
+      <c r="N19">
+        <v>2500</v>
+      </c>
+      <c r="O19">
+        <v>2500</v>
+      </c>
+      <c r="P19">
+        <v>2500</v>
+      </c>
+      <c r="Q19">
+        <v>2500</v>
+      </c>
+      <c r="R19">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>123</v>
+      </c>
+      <c r="B20" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20">
+        <v>3200</v>
+      </c>
+      <c r="D20">
+        <v>3200</v>
+      </c>
+      <c r="E20">
+        <v>3200</v>
+      </c>
+      <c r="F20">
+        <v>3200</v>
+      </c>
+      <c r="G20">
+        <v>3200</v>
+      </c>
+      <c r="H20">
+        <v>3200</v>
+      </c>
+      <c r="I20">
+        <v>3200</v>
+      </c>
+      <c r="J20">
+        <v>3200</v>
+      </c>
+      <c r="K20">
+        <v>3200</v>
+      </c>
+      <c r="L20">
+        <v>3200</v>
+      </c>
+      <c r="M20">
+        <v>3200</v>
+      </c>
+      <c r="N20">
+        <v>3200</v>
+      </c>
+      <c r="O20">
+        <v>3200</v>
+      </c>
+      <c r="P20">
+        <v>3200</v>
+      </c>
+      <c r="Q20">
+        <v>3200</v>
+      </c>
+      <c r="R20">
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>124</v>
+      </c>
+      <c r="B21" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21">
+        <v>3200</v>
+      </c>
+      <c r="D21">
+        <v>3200</v>
+      </c>
+      <c r="E21">
+        <v>3200</v>
+      </c>
+      <c r="F21">
+        <v>3200</v>
+      </c>
+      <c r="G21">
+        <v>3200</v>
+      </c>
+      <c r="H21">
+        <v>3200</v>
+      </c>
+      <c r="I21">
+        <v>3200</v>
+      </c>
+      <c r="J21">
+        <v>3200</v>
+      </c>
+      <c r="K21">
+        <v>3200</v>
+      </c>
+      <c r="L21">
+        <v>3200</v>
+      </c>
+      <c r="M21">
+        <v>3200</v>
+      </c>
+      <c r="N21">
+        <v>3200</v>
+      </c>
+      <c r="O21">
+        <v>3200</v>
+      </c>
+      <c r="P21">
+        <v>3200</v>
+      </c>
+      <c r="Q21">
+        <v>3200</v>
+      </c>
+      <c r="R21">
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>125</v>
+      </c>
+      <c r="B22" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22">
+        <v>3200</v>
+      </c>
+      <c r="D22">
+        <v>3200</v>
+      </c>
+      <c r="E22">
+        <v>3200</v>
+      </c>
+      <c r="F22">
+        <v>3200</v>
+      </c>
+      <c r="G22">
+        <v>3200</v>
+      </c>
+      <c r="H22">
+        <v>3200</v>
+      </c>
+      <c r="I22">
+        <v>3200</v>
+      </c>
+      <c r="J22">
+        <v>3200</v>
+      </c>
+      <c r="K22">
+        <v>3200</v>
+      </c>
+      <c r="L22">
+        <v>3200</v>
+      </c>
+      <c r="M22">
+        <v>3200</v>
+      </c>
+      <c r="N22">
+        <v>3200</v>
+      </c>
+      <c r="O22">
+        <v>3200</v>
+      </c>
+      <c r="P22">
+        <v>3200</v>
+      </c>
+      <c r="Q22">
+        <v>3200</v>
+      </c>
+      <c r="R22">
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>126</v>
       </c>
-      <c r="B20" t="s">
-        <v>62</v>
-      </c>
-      <c r="C20" t="s">
-        <v>58</v>
-      </c>
-      <c r="D20" t="s">
-        <v>77</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="F20">
-        <v>3200</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>127</v>
-      </c>
-      <c r="B21" t="s">
-        <v>62</v>
-      </c>
-      <c r="C21" t="s">
-        <v>58</v>
-      </c>
-      <c r="D21" t="s">
-        <v>78</v>
-      </c>
-      <c r="E21">
-        <v>2</v>
-      </c>
-      <c r="F21">
-        <v>3200</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>128</v>
-      </c>
-      <c r="B22" t="s">
-        <v>62</v>
-      </c>
-      <c r="C22" t="s">
-        <v>58</v>
-      </c>
-      <c r="D22" t="s">
-        <v>79</v>
-      </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-      <c r="F22">
-        <v>3200</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>129</v>
-      </c>
       <c r="B23" t="s">
-        <v>54</v>
-      </c>
-      <c r="C23" t="s">
-        <v>55</v>
-      </c>
-      <c r="D23" t="s">
         <v>80</v>
       </c>
+      <c r="C23">
+        <v>28</v>
+      </c>
+      <c r="D23">
+        <v>28</v>
+      </c>
       <c r="E23">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="F23">
         <v>28</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G23">
+        <v>28</v>
+      </c>
+      <c r="H23">
+        <v>28</v>
+      </c>
+      <c r="I23">
+        <v>28</v>
+      </c>
+      <c r="J23">
+        <v>28</v>
+      </c>
+      <c r="K23">
+        <v>28</v>
+      </c>
+      <c r="L23">
+        <v>28</v>
+      </c>
+      <c r="M23">
+        <v>28</v>
+      </c>
+      <c r="N23">
+        <v>28</v>
+      </c>
+      <c r="O23">
+        <v>28</v>
+      </c>
+      <c r="P23">
+        <v>28</v>
+      </c>
+      <c r="Q23">
+        <v>28</v>
+      </c>
+      <c r="R23">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B24" t="s">
-        <v>66</v>
-      </c>
-      <c r="C24" t="s">
-        <v>55</v>
-      </c>
-      <c r="D24" t="s">
         <v>81</v>
       </c>
+      <c r="C24">
+        <v>50</v>
+      </c>
+      <c r="D24">
+        <v>50</v>
+      </c>
       <c r="E24">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="F24">
         <v>50</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G24">
+        <v>50</v>
+      </c>
+      <c r="H24">
+        <v>50</v>
+      </c>
+      <c r="I24">
+        <v>50</v>
+      </c>
+      <c r="J24">
+        <v>50</v>
+      </c>
+      <c r="K24">
+        <v>50</v>
+      </c>
+      <c r="L24">
+        <v>50</v>
+      </c>
+      <c r="M24">
+        <v>50</v>
+      </c>
+      <c r="N24">
+        <v>50</v>
+      </c>
+      <c r="O24">
+        <v>50</v>
+      </c>
+      <c r="P24">
+        <v>50</v>
+      </c>
+      <c r="Q24">
+        <v>50</v>
+      </c>
+      <c r="R24">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B25" t="s">
-        <v>54</v>
-      </c>
-      <c r="C25" t="s">
-        <v>55</v>
-      </c>
-      <c r="D25" t="s">
         <v>82</v>
       </c>
+      <c r="C25">
+        <v>32</v>
+      </c>
+      <c r="D25">
+        <v>32</v>
+      </c>
       <c r="E25">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="F25">
         <v>32</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G25">
+        <v>32</v>
+      </c>
+      <c r="H25">
+        <v>32</v>
+      </c>
+      <c r="I25">
+        <v>32</v>
+      </c>
+      <c r="J25">
+        <v>32</v>
+      </c>
+      <c r="K25">
+        <v>32</v>
+      </c>
+      <c r="L25">
+        <v>32</v>
+      </c>
+      <c r="M25">
+        <v>32</v>
+      </c>
+      <c r="N25">
+        <v>32</v>
+      </c>
+      <c r="O25">
+        <v>32</v>
+      </c>
+      <c r="P25">
+        <v>32</v>
+      </c>
+      <c r="Q25">
+        <v>32</v>
+      </c>
+      <c r="R25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>104</v>
+      </c>
+      <c r="B26" t="s">
+        <v>83</v>
+      </c>
+      <c r="C26">
+        <v>30</v>
+      </c>
+      <c r="D26">
+        <v>30</v>
+      </c>
+      <c r="E26">
+        <v>30</v>
+      </c>
+      <c r="F26">
+        <v>30</v>
+      </c>
+      <c r="G26">
+        <v>30</v>
+      </c>
+      <c r="H26">
+        <v>30</v>
+      </c>
+      <c r="I26">
+        <v>30</v>
+      </c>
+      <c r="J26">
+        <v>30</v>
+      </c>
+      <c r="K26">
+        <v>30</v>
+      </c>
+      <c r="L26">
+        <v>30</v>
+      </c>
+      <c r="M26">
+        <v>30</v>
+      </c>
+      <c r="N26">
+        <v>30</v>
+      </c>
+      <c r="O26">
+        <v>30</v>
+      </c>
+      <c r="P26">
+        <v>30</v>
+      </c>
+      <c r="Q26">
+        <v>30</v>
+      </c>
+      <c r="R26">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A4EACD5-3DDB-4A06-AA6C-C8F9511D9F67}">
+  <dimension ref="A1:R26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="18" width="7.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2023</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2024</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2025</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2026</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2027</v>
+      </c>
+      <c r="K1" s="1">
+        <v>2028</v>
+      </c>
+      <c r="L1" s="1">
+        <v>2029</v>
+      </c>
+      <c r="M1" s="1">
+        <v>2030</v>
+      </c>
+      <c r="N1" s="1">
+        <v>2031</v>
+      </c>
+      <c r="O1" s="1">
+        <v>2032</v>
+      </c>
+      <c r="P1" s="1">
+        <v>2033</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>2034</v>
+      </c>
+      <c r="R1" s="1">
+        <v>2035</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2">
+        <v>20</v>
+      </c>
+      <c r="D2">
+        <v>20</v>
+      </c>
+      <c r="E2">
+        <v>20</v>
+      </c>
+      <c r="F2">
+        <v>20</v>
+      </c>
+      <c r="G2">
+        <v>20</v>
+      </c>
+      <c r="H2">
+        <v>20</v>
+      </c>
+      <c r="I2">
+        <v>20</v>
+      </c>
+      <c r="J2">
+        <v>20</v>
+      </c>
+      <c r="K2">
+        <v>20</v>
+      </c>
+      <c r="L2">
+        <v>20</v>
+      </c>
+      <c r="M2">
+        <v>20</v>
+      </c>
+      <c r="N2">
+        <v>20</v>
+      </c>
+      <c r="O2">
+        <v>20</v>
+      </c>
+      <c r="P2">
+        <v>20</v>
+      </c>
+      <c r="Q2">
+        <v>20</v>
+      </c>
+      <c r="R2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3">
+        <v>18</v>
+      </c>
+      <c r="D3">
+        <v>18</v>
+      </c>
+      <c r="E3">
+        <v>18</v>
+      </c>
+      <c r="F3">
+        <v>18</v>
+      </c>
+      <c r="G3">
+        <v>18</v>
+      </c>
+      <c r="H3">
+        <v>18</v>
+      </c>
+      <c r="I3">
+        <v>18</v>
+      </c>
+      <c r="J3">
+        <v>18</v>
+      </c>
+      <c r="K3">
+        <v>18</v>
+      </c>
+      <c r="L3">
+        <v>18</v>
+      </c>
+      <c r="M3">
+        <v>18</v>
+      </c>
+      <c r="N3">
+        <v>18</v>
+      </c>
+      <c r="O3">
+        <v>18</v>
+      </c>
+      <c r="P3">
+        <v>18</v>
+      </c>
+      <c r="Q3">
+        <v>18</v>
+      </c>
+      <c r="R3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>107</v>
       </c>
+      <c r="B4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4">
+        <v>390</v>
+      </c>
+      <c r="D4">
+        <v>390</v>
+      </c>
+      <c r="E4">
+        <v>390</v>
+      </c>
+      <c r="F4">
+        <v>390</v>
+      </c>
+      <c r="G4">
+        <v>390</v>
+      </c>
+      <c r="H4">
+        <v>390</v>
+      </c>
+      <c r="I4">
+        <v>390</v>
+      </c>
+      <c r="J4">
+        <v>390</v>
+      </c>
+      <c r="K4">
+        <v>390</v>
+      </c>
+      <c r="L4">
+        <v>390</v>
+      </c>
+      <c r="M4">
+        <v>390</v>
+      </c>
+      <c r="N4">
+        <v>390</v>
+      </c>
+      <c r="O4">
+        <v>390</v>
+      </c>
+      <c r="P4">
+        <v>390</v>
+      </c>
+      <c r="Q4">
+        <v>390</v>
+      </c>
+      <c r="R4">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5">
+        <v>390</v>
+      </c>
+      <c r="D5">
+        <v>390</v>
+      </c>
+      <c r="E5">
+        <v>390</v>
+      </c>
+      <c r="F5">
+        <v>390</v>
+      </c>
+      <c r="G5">
+        <v>390</v>
+      </c>
+      <c r="H5">
+        <v>390</v>
+      </c>
+      <c r="I5">
+        <v>390</v>
+      </c>
+      <c r="J5">
+        <v>390</v>
+      </c>
+      <c r="K5">
+        <v>390</v>
+      </c>
+      <c r="L5">
+        <v>390</v>
+      </c>
+      <c r="M5">
+        <v>390</v>
+      </c>
+      <c r="N5">
+        <v>390</v>
+      </c>
+      <c r="O5">
+        <v>390</v>
+      </c>
+      <c r="P5">
+        <v>390</v>
+      </c>
+      <c r="Q5">
+        <v>390</v>
+      </c>
+      <c r="R5">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6">
+        <v>390</v>
+      </c>
+      <c r="D6">
+        <v>390</v>
+      </c>
+      <c r="E6">
+        <v>390</v>
+      </c>
+      <c r="F6">
+        <v>390</v>
+      </c>
+      <c r="G6">
+        <v>390</v>
+      </c>
+      <c r="H6">
+        <v>390</v>
+      </c>
+      <c r="I6">
+        <v>390</v>
+      </c>
+      <c r="J6">
+        <v>390</v>
+      </c>
+      <c r="K6">
+        <v>390</v>
+      </c>
+      <c r="L6">
+        <v>390</v>
+      </c>
+      <c r="M6">
+        <v>390</v>
+      </c>
+      <c r="N6">
+        <v>390</v>
+      </c>
+      <c r="O6">
+        <v>390</v>
+      </c>
+      <c r="P6">
+        <v>390</v>
+      </c>
+      <c r="Q6">
+        <v>390</v>
+      </c>
+      <c r="R6">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>110</v>
+      </c>
+      <c r="B7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7">
+        <v>3000</v>
+      </c>
+      <c r="D7">
+        <v>3000</v>
+      </c>
+      <c r="E7">
+        <v>3000</v>
+      </c>
+      <c r="F7">
+        <v>3000</v>
+      </c>
+      <c r="G7">
+        <v>3000</v>
+      </c>
+      <c r="H7">
+        <v>3000</v>
+      </c>
+      <c r="I7">
+        <v>3000</v>
+      </c>
+      <c r="J7">
+        <v>3000</v>
+      </c>
+      <c r="K7">
+        <v>3000</v>
+      </c>
+      <c r="L7">
+        <v>3000</v>
+      </c>
+      <c r="M7">
+        <v>3000</v>
+      </c>
+      <c r="N7">
+        <v>3000</v>
+      </c>
+      <c r="O7">
+        <v>3000</v>
+      </c>
+      <c r="P7">
+        <v>3000</v>
+      </c>
+      <c r="Q7">
+        <v>3000</v>
+      </c>
+      <c r="R7">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8">
+        <v>3000</v>
+      </c>
+      <c r="D8">
+        <v>3000</v>
+      </c>
+      <c r="E8">
+        <v>3000</v>
+      </c>
+      <c r="F8">
+        <v>3000</v>
+      </c>
+      <c r="G8">
+        <v>3000</v>
+      </c>
+      <c r="H8">
+        <v>3000</v>
+      </c>
+      <c r="I8">
+        <v>3000</v>
+      </c>
+      <c r="J8">
+        <v>3000</v>
+      </c>
+      <c r="K8">
+        <v>3000</v>
+      </c>
+      <c r="L8">
+        <v>3000</v>
+      </c>
+      <c r="M8">
+        <v>3000</v>
+      </c>
+      <c r="N8">
+        <v>3000</v>
+      </c>
+      <c r="O8">
+        <v>3000</v>
+      </c>
+      <c r="P8">
+        <v>3000</v>
+      </c>
+      <c r="Q8">
+        <v>3000</v>
+      </c>
+      <c r="R8">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9">
+        <v>3000</v>
+      </c>
+      <c r="D9">
+        <v>3000</v>
+      </c>
+      <c r="E9">
+        <v>3000</v>
+      </c>
+      <c r="F9">
+        <v>3000</v>
+      </c>
+      <c r="G9">
+        <v>3000</v>
+      </c>
+      <c r="H9">
+        <v>3000</v>
+      </c>
+      <c r="I9">
+        <v>3000</v>
+      </c>
+      <c r="J9">
+        <v>3000</v>
+      </c>
+      <c r="K9">
+        <v>3000</v>
+      </c>
+      <c r="L9">
+        <v>3000</v>
+      </c>
+      <c r="M9">
+        <v>3000</v>
+      </c>
+      <c r="N9">
+        <v>3000</v>
+      </c>
+      <c r="O9">
+        <v>3000</v>
+      </c>
+      <c r="P9">
+        <v>3000</v>
+      </c>
+      <c r="Q9">
+        <v>3000</v>
+      </c>
+      <c r="R9">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>113</v>
+      </c>
+      <c r="B10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10">
+        <v>75</v>
+      </c>
+      <c r="D10">
+        <v>75</v>
+      </c>
+      <c r="E10">
+        <v>75</v>
+      </c>
+      <c r="F10">
+        <v>75</v>
+      </c>
+      <c r="G10">
+        <v>75</v>
+      </c>
+      <c r="H10">
+        <v>75</v>
+      </c>
+      <c r="I10">
+        <v>75</v>
+      </c>
+      <c r="J10">
+        <v>75</v>
+      </c>
+      <c r="K10">
+        <v>75</v>
+      </c>
+      <c r="L10">
+        <v>75</v>
+      </c>
+      <c r="M10">
+        <v>75</v>
+      </c>
+      <c r="N10">
+        <v>75</v>
+      </c>
+      <c r="O10">
+        <v>75</v>
+      </c>
+      <c r="P10">
+        <v>75</v>
+      </c>
+      <c r="Q10">
+        <v>75</v>
+      </c>
+      <c r="R10">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11">
+        <v>40</v>
+      </c>
+      <c r="D11">
+        <v>40</v>
+      </c>
+      <c r="E11">
+        <v>40</v>
+      </c>
+      <c r="F11">
+        <v>40</v>
+      </c>
+      <c r="G11">
+        <v>40</v>
+      </c>
+      <c r="H11">
+        <v>40</v>
+      </c>
+      <c r="I11">
+        <v>40</v>
+      </c>
+      <c r="J11">
+        <v>40</v>
+      </c>
+      <c r="K11">
+        <v>40</v>
+      </c>
+      <c r="L11">
+        <v>40</v>
+      </c>
+      <c r="M11">
+        <v>40</v>
+      </c>
+      <c r="N11">
+        <v>40</v>
+      </c>
+      <c r="O11">
+        <v>40</v>
+      </c>
+      <c r="P11">
+        <v>40</v>
+      </c>
+      <c r="Q11">
+        <v>40</v>
+      </c>
+      <c r="R11">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>115</v>
+      </c>
+      <c r="B12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12">
+        <v>330</v>
+      </c>
+      <c r="D12">
+        <v>330</v>
+      </c>
+      <c r="E12">
+        <v>330</v>
+      </c>
+      <c r="F12">
+        <v>330</v>
+      </c>
+      <c r="G12">
+        <v>330</v>
+      </c>
+      <c r="H12">
+        <v>330</v>
+      </c>
+      <c r="I12">
+        <v>330</v>
+      </c>
+      <c r="J12">
+        <v>330</v>
+      </c>
+      <c r="K12">
+        <v>330</v>
+      </c>
+      <c r="L12">
+        <v>330</v>
+      </c>
+      <c r="M12">
+        <v>330</v>
+      </c>
+      <c r="N12">
+        <v>330</v>
+      </c>
+      <c r="O12">
+        <v>330</v>
+      </c>
+      <c r="P12">
+        <v>330</v>
+      </c>
+      <c r="Q12">
+        <v>330</v>
+      </c>
+      <c r="R12">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>116</v>
+      </c>
+      <c r="B13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13">
+        <v>330</v>
+      </c>
+      <c r="D13">
+        <v>330</v>
+      </c>
+      <c r="E13">
+        <v>330</v>
+      </c>
+      <c r="F13">
+        <v>330</v>
+      </c>
+      <c r="G13">
+        <v>330</v>
+      </c>
+      <c r="H13">
+        <v>330</v>
+      </c>
+      <c r="I13">
+        <v>330</v>
+      </c>
+      <c r="J13">
+        <v>330</v>
+      </c>
+      <c r="K13">
+        <v>330</v>
+      </c>
+      <c r="L13">
+        <v>330</v>
+      </c>
+      <c r="M13">
+        <v>330</v>
+      </c>
+      <c r="N13">
+        <v>330</v>
+      </c>
+      <c r="O13">
+        <v>330</v>
+      </c>
+      <c r="P13">
+        <v>330</v>
+      </c>
+      <c r="Q13">
+        <v>330</v>
+      </c>
+      <c r="R13">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>117</v>
+      </c>
+      <c r="B14" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14">
+        <v>330</v>
+      </c>
+      <c r="D14">
+        <v>330</v>
+      </c>
+      <c r="E14">
+        <v>330</v>
+      </c>
+      <c r="F14">
+        <v>330</v>
+      </c>
+      <c r="G14">
+        <v>330</v>
+      </c>
+      <c r="H14">
+        <v>330</v>
+      </c>
+      <c r="I14">
+        <v>330</v>
+      </c>
+      <c r="J14">
+        <v>330</v>
+      </c>
+      <c r="K14">
+        <v>330</v>
+      </c>
+      <c r="L14">
+        <v>330</v>
+      </c>
+      <c r="M14">
+        <v>330</v>
+      </c>
+      <c r="N14">
+        <v>330</v>
+      </c>
+      <c r="O14">
+        <v>330</v>
+      </c>
+      <c r="P14">
+        <v>330</v>
+      </c>
+      <c r="Q14">
+        <v>330</v>
+      </c>
+      <c r="R14">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>118</v>
+      </c>
+      <c r="B15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15">
+        <v>75</v>
+      </c>
+      <c r="D15">
+        <v>75</v>
+      </c>
+      <c r="E15">
+        <v>75</v>
+      </c>
+      <c r="F15">
+        <v>75</v>
+      </c>
+      <c r="G15">
+        <v>75</v>
+      </c>
+      <c r="H15">
+        <v>75</v>
+      </c>
+      <c r="I15">
+        <v>75</v>
+      </c>
+      <c r="J15">
+        <v>75</v>
+      </c>
+      <c r="K15">
+        <v>75</v>
+      </c>
+      <c r="L15">
+        <v>75</v>
+      </c>
+      <c r="M15">
+        <v>75</v>
+      </c>
+      <c r="N15">
+        <v>75</v>
+      </c>
+      <c r="O15">
+        <v>75</v>
+      </c>
+      <c r="P15">
+        <v>75</v>
+      </c>
+      <c r="Q15">
+        <v>75</v>
+      </c>
+      <c r="R15">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>119</v>
+      </c>
+      <c r="B16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16">
+        <v>50</v>
+      </c>
+      <c r="D16">
+        <v>50</v>
+      </c>
+      <c r="E16">
+        <v>50</v>
+      </c>
+      <c r="F16">
+        <v>50</v>
+      </c>
+      <c r="G16">
+        <v>50</v>
+      </c>
+      <c r="H16">
+        <v>50</v>
+      </c>
+      <c r="I16">
+        <v>50</v>
+      </c>
+      <c r="J16">
+        <v>50</v>
+      </c>
+      <c r="K16">
+        <v>50</v>
+      </c>
+      <c r="L16">
+        <v>50</v>
+      </c>
+      <c r="M16">
+        <v>50</v>
+      </c>
+      <c r="N16">
+        <v>50</v>
+      </c>
+      <c r="O16">
+        <v>50</v>
+      </c>
+      <c r="P16">
+        <v>50</v>
+      </c>
+      <c r="Q16">
+        <v>50</v>
+      </c>
+      <c r="R16">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>120</v>
+      </c>
+      <c r="B17" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17">
+        <v>250</v>
+      </c>
+      <c r="D17">
+        <v>250</v>
+      </c>
+      <c r="E17">
+        <v>250</v>
+      </c>
+      <c r="F17">
+        <v>250</v>
+      </c>
+      <c r="G17">
+        <v>250</v>
+      </c>
+      <c r="H17">
+        <v>250</v>
+      </c>
+      <c r="I17">
+        <v>250</v>
+      </c>
+      <c r="J17">
+        <v>250</v>
+      </c>
+      <c r="K17">
+        <v>250</v>
+      </c>
+      <c r="L17">
+        <v>250</v>
+      </c>
+      <c r="M17">
+        <v>250</v>
+      </c>
+      <c r="N17">
+        <v>250</v>
+      </c>
+      <c r="O17">
+        <v>250</v>
+      </c>
+      <c r="P17">
+        <v>250</v>
+      </c>
+      <c r="Q17">
+        <v>250</v>
+      </c>
+      <c r="R17">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>121</v>
+      </c>
+      <c r="B18" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18">
+        <v>2400</v>
+      </c>
+      <c r="D18">
+        <v>2400</v>
+      </c>
+      <c r="E18">
+        <v>2400</v>
+      </c>
+      <c r="F18">
+        <v>2400</v>
+      </c>
+      <c r="G18">
+        <v>2400</v>
+      </c>
+      <c r="H18">
+        <v>2400</v>
+      </c>
+      <c r="I18">
+        <v>2400</v>
+      </c>
+      <c r="J18">
+        <v>2400</v>
+      </c>
+      <c r="K18">
+        <v>2400</v>
+      </c>
+      <c r="L18">
+        <v>2400</v>
+      </c>
+      <c r="M18">
+        <v>2400</v>
+      </c>
+      <c r="N18">
+        <v>2400</v>
+      </c>
+      <c r="O18">
+        <v>2400</v>
+      </c>
+      <c r="P18">
+        <v>2400</v>
+      </c>
+      <c r="Q18">
+        <v>2400</v>
+      </c>
+      <c r="R18">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>122</v>
+      </c>
+      <c r="B19" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19">
+        <v>2500</v>
+      </c>
+      <c r="D19">
+        <v>2500</v>
+      </c>
+      <c r="E19">
+        <v>2500</v>
+      </c>
+      <c r="F19">
+        <v>2500</v>
+      </c>
+      <c r="G19">
+        <v>2500</v>
+      </c>
+      <c r="H19">
+        <v>2500</v>
+      </c>
+      <c r="I19">
+        <v>2500</v>
+      </c>
+      <c r="J19">
+        <v>2500</v>
+      </c>
+      <c r="K19">
+        <v>2500</v>
+      </c>
+      <c r="L19">
+        <v>2500</v>
+      </c>
+      <c r="M19">
+        <v>2500</v>
+      </c>
+      <c r="N19">
+        <v>2500</v>
+      </c>
+      <c r="O19">
+        <v>2500</v>
+      </c>
+      <c r="P19">
+        <v>2500</v>
+      </c>
+      <c r="Q19">
+        <v>2500</v>
+      </c>
+      <c r="R19">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>123</v>
+      </c>
+      <c r="B20" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20">
+        <v>3200</v>
+      </c>
+      <c r="D20">
+        <v>3200</v>
+      </c>
+      <c r="E20">
+        <v>3200</v>
+      </c>
+      <c r="F20">
+        <v>3200</v>
+      </c>
+      <c r="G20">
+        <v>3200</v>
+      </c>
+      <c r="H20">
+        <v>3200</v>
+      </c>
+      <c r="I20">
+        <v>3200</v>
+      </c>
+      <c r="J20">
+        <v>3200</v>
+      </c>
+      <c r="K20">
+        <v>3200</v>
+      </c>
+      <c r="L20">
+        <v>3200</v>
+      </c>
+      <c r="M20">
+        <v>3200</v>
+      </c>
+      <c r="N20">
+        <v>3200</v>
+      </c>
+      <c r="O20">
+        <v>3200</v>
+      </c>
+      <c r="P20">
+        <v>3200</v>
+      </c>
+      <c r="Q20">
+        <v>3200</v>
+      </c>
+      <c r="R20">
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>124</v>
+      </c>
+      <c r="B21" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21">
+        <v>3200</v>
+      </c>
+      <c r="D21">
+        <v>3200</v>
+      </c>
+      <c r="E21">
+        <v>3200</v>
+      </c>
+      <c r="F21">
+        <v>3200</v>
+      </c>
+      <c r="G21">
+        <v>3200</v>
+      </c>
+      <c r="H21">
+        <v>3200</v>
+      </c>
+      <c r="I21">
+        <v>3200</v>
+      </c>
+      <c r="J21">
+        <v>3200</v>
+      </c>
+      <c r="K21">
+        <v>3200</v>
+      </c>
+      <c r="L21">
+        <v>3200</v>
+      </c>
+      <c r="M21">
+        <v>3200</v>
+      </c>
+      <c r="N21">
+        <v>3200</v>
+      </c>
+      <c r="O21">
+        <v>3200</v>
+      </c>
+      <c r="P21">
+        <v>3200</v>
+      </c>
+      <c r="Q21">
+        <v>3200</v>
+      </c>
+      <c r="R21">
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>125</v>
+      </c>
+      <c r="B22" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22">
+        <v>3200</v>
+      </c>
+      <c r="D22">
+        <v>3200</v>
+      </c>
+      <c r="E22">
+        <v>3200</v>
+      </c>
+      <c r="F22">
+        <v>3200</v>
+      </c>
+      <c r="G22">
+        <v>3200</v>
+      </c>
+      <c r="H22">
+        <v>3200</v>
+      </c>
+      <c r="I22">
+        <v>3200</v>
+      </c>
+      <c r="J22">
+        <v>3200</v>
+      </c>
+      <c r="K22">
+        <v>3200</v>
+      </c>
+      <c r="L22">
+        <v>3200</v>
+      </c>
+      <c r="M22">
+        <v>3200</v>
+      </c>
+      <c r="N22">
+        <v>3200</v>
+      </c>
+      <c r="O22">
+        <v>3200</v>
+      </c>
+      <c r="P22">
+        <v>3200</v>
+      </c>
+      <c r="Q22">
+        <v>3200</v>
+      </c>
+      <c r="R22">
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>126</v>
+      </c>
+      <c r="B23" t="s">
+        <v>80</v>
+      </c>
+      <c r="C23">
+        <v>28</v>
+      </c>
+      <c r="D23">
+        <v>28</v>
+      </c>
+      <c r="E23">
+        <v>28</v>
+      </c>
+      <c r="F23">
+        <v>28</v>
+      </c>
+      <c r="G23">
+        <v>28</v>
+      </c>
+      <c r="H23">
+        <v>28</v>
+      </c>
+      <c r="I23">
+        <v>28</v>
+      </c>
+      <c r="J23">
+        <v>28</v>
+      </c>
+      <c r="K23">
+        <v>28</v>
+      </c>
+      <c r="L23">
+        <v>28</v>
+      </c>
+      <c r="M23">
+        <v>28</v>
+      </c>
+      <c r="N23">
+        <v>28</v>
+      </c>
+      <c r="O23">
+        <v>28</v>
+      </c>
+      <c r="P23">
+        <v>28</v>
+      </c>
+      <c r="Q23">
+        <v>28</v>
+      </c>
+      <c r="R23">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>102</v>
+      </c>
+      <c r="B24" t="s">
+        <v>81</v>
+      </c>
+      <c r="C24">
+        <v>50</v>
+      </c>
+      <c r="D24">
+        <v>50</v>
+      </c>
+      <c r="E24">
+        <v>50</v>
+      </c>
+      <c r="F24">
+        <v>50</v>
+      </c>
+      <c r="G24">
+        <v>50</v>
+      </c>
+      <c r="H24">
+        <v>50</v>
+      </c>
+      <c r="I24">
+        <v>50</v>
+      </c>
+      <c r="J24">
+        <v>50</v>
+      </c>
+      <c r="K24">
+        <v>50</v>
+      </c>
+      <c r="L24">
+        <v>50</v>
+      </c>
+      <c r="M24">
+        <v>50</v>
+      </c>
+      <c r="N24">
+        <v>50</v>
+      </c>
+      <c r="O24">
+        <v>50</v>
+      </c>
+      <c r="P24">
+        <v>50</v>
+      </c>
+      <c r="Q24">
+        <v>50</v>
+      </c>
+      <c r="R24">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>103</v>
+      </c>
+      <c r="B25" t="s">
+        <v>82</v>
+      </c>
+      <c r="C25">
+        <v>32</v>
+      </c>
+      <c r="D25">
+        <v>32</v>
+      </c>
+      <c r="E25">
+        <v>32</v>
+      </c>
+      <c r="F25">
+        <v>32</v>
+      </c>
+      <c r="G25">
+        <v>32</v>
+      </c>
+      <c r="H25">
+        <v>32</v>
+      </c>
+      <c r="I25">
+        <v>32</v>
+      </c>
+      <c r="J25">
+        <v>32</v>
+      </c>
+      <c r="K25">
+        <v>32</v>
+      </c>
+      <c r="L25">
+        <v>32</v>
+      </c>
+      <c r="M25">
+        <v>32</v>
+      </c>
+      <c r="N25">
+        <v>32</v>
+      </c>
+      <c r="O25">
+        <v>32</v>
+      </c>
+      <c r="P25">
+        <v>32</v>
+      </c>
+      <c r="Q25">
+        <v>32</v>
+      </c>
+      <c r="R25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>104</v>
+      </c>
       <c r="B26" t="s">
-        <v>54</v>
-      </c>
-      <c r="C26" t="s">
-        <v>55</v>
-      </c>
-      <c r="D26" t="s">
         <v>83</v>
       </c>
+      <c r="C26">
+        <v>30</v>
+      </c>
+      <c r="D26">
+        <v>30</v>
+      </c>
       <c r="E26">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="F26">
+        <v>30</v>
+      </c>
+      <c r="G26">
+        <v>30</v>
+      </c>
+      <c r="H26">
+        <v>30</v>
+      </c>
+      <c r="I26">
+        <v>30</v>
+      </c>
+      <c r="J26">
+        <v>30</v>
+      </c>
+      <c r="K26">
+        <v>30</v>
+      </c>
+      <c r="L26">
+        <v>30</v>
+      </c>
+      <c r="M26">
+        <v>30</v>
+      </c>
+      <c r="N26">
+        <v>30</v>
+      </c>
+      <c r="O26">
+        <v>30</v>
+      </c>
+      <c r="P26">
+        <v>30</v>
+      </c>
+      <c r="Q26">
+        <v>30</v>
+      </c>
+      <c r="R26">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
import prices tested on A03
</commit_message>
<xml_diff>
--- a/generator/masterdata.xlsx
+++ b/generator/masterdata.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F0DFD6C-DE74-4E19-8C23-FF9C12738E41}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D138FFAD-B52C-495B-95B3-C0501B09BD48}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="10500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="10500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="years" sheetId="7" r:id="rId1"/>
@@ -14,6 +14,7 @@
     <sheet name="materials" sheetId="2" r:id="rId4"/>
     <sheet name="prices EUR" sheetId="5" r:id="rId5"/>
     <sheet name="prices USD" sheetId="6" r:id="rId6"/>
+    <sheet name="customers x materials" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="129">
   <si>
     <t>Rocky Mountain Bikes</t>
   </si>
@@ -467,7 +468,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -475,6 +476,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -758,7 +760,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23D9E596-51CC-440C-8BFE-8B4B0D6F8F00}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1360,9 +1362,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1961,7 +1961,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5367,4 +5367,2023 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95ED7805-F9C9-44B5-8A0B-A5E579593692}">
+  <dimension ref="A1:Z25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+      <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2">
+        <v>1</v>
+      </c>
+      <c r="W2">
+        <v>1</v>
+      </c>
+      <c r="X2">
+        <v>1</v>
+      </c>
+      <c r="Y2">
+        <v>1</v>
+      </c>
+      <c r="Z2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <v>1</v>
+      </c>
+      <c r="U3">
+        <v>1</v>
+      </c>
+      <c r="V3">
+        <v>1</v>
+      </c>
+      <c r="W3">
+        <v>1</v>
+      </c>
+      <c r="X3">
+        <v>1</v>
+      </c>
+      <c r="Y3">
+        <v>1</v>
+      </c>
+      <c r="Z3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="R4">
+        <v>1</v>
+      </c>
+      <c r="S4">
+        <v>1</v>
+      </c>
+      <c r="T4">
+        <v>1</v>
+      </c>
+      <c r="U4">
+        <v>1</v>
+      </c>
+      <c r="V4">
+        <v>1</v>
+      </c>
+      <c r="W4">
+        <v>1</v>
+      </c>
+      <c r="X4">
+        <v>1</v>
+      </c>
+      <c r="Y4">
+        <v>1</v>
+      </c>
+      <c r="Z4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="S5">
+        <v>1</v>
+      </c>
+      <c r="T5">
+        <v>1</v>
+      </c>
+      <c r="U5">
+        <v>1</v>
+      </c>
+      <c r="V5">
+        <v>1</v>
+      </c>
+      <c r="W5">
+        <v>1</v>
+      </c>
+      <c r="X5">
+        <v>1</v>
+      </c>
+      <c r="Y5">
+        <v>1</v>
+      </c>
+      <c r="Z5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <v>1</v>
+      </c>
+      <c r="T6">
+        <v>1</v>
+      </c>
+      <c r="U6">
+        <v>1</v>
+      </c>
+      <c r="V6">
+        <v>1</v>
+      </c>
+      <c r="W6">
+        <v>1</v>
+      </c>
+      <c r="X6">
+        <v>1</v>
+      </c>
+      <c r="Y6">
+        <v>1</v>
+      </c>
+      <c r="Z6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+      <c r="R7">
+        <v>1</v>
+      </c>
+      <c r="S7">
+        <v>1</v>
+      </c>
+      <c r="T7">
+        <v>1</v>
+      </c>
+      <c r="U7">
+        <v>1</v>
+      </c>
+      <c r="V7">
+        <v>1</v>
+      </c>
+      <c r="W7">
+        <v>1</v>
+      </c>
+      <c r="X7">
+        <v>1</v>
+      </c>
+      <c r="Y7">
+        <v>1</v>
+      </c>
+      <c r="Z7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <v>1</v>
+      </c>
+      <c r="S8">
+        <v>1</v>
+      </c>
+      <c r="T8">
+        <v>1</v>
+      </c>
+      <c r="U8">
+        <v>1</v>
+      </c>
+      <c r="V8">
+        <v>1</v>
+      </c>
+      <c r="W8">
+        <v>1</v>
+      </c>
+      <c r="X8">
+        <v>1</v>
+      </c>
+      <c r="Y8">
+        <v>1</v>
+      </c>
+      <c r="Z8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9">
+        <v>1</v>
+      </c>
+      <c r="Q9">
+        <v>1</v>
+      </c>
+      <c r="R9">
+        <v>1</v>
+      </c>
+      <c r="S9">
+        <v>1</v>
+      </c>
+      <c r="T9">
+        <v>1</v>
+      </c>
+      <c r="U9">
+        <v>1</v>
+      </c>
+      <c r="V9">
+        <v>1</v>
+      </c>
+      <c r="W9">
+        <v>1</v>
+      </c>
+      <c r="X9">
+        <v>1</v>
+      </c>
+      <c r="Y9">
+        <v>1</v>
+      </c>
+      <c r="Z9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+      <c r="Q10">
+        <v>1</v>
+      </c>
+      <c r="R10">
+        <v>1</v>
+      </c>
+      <c r="S10">
+        <v>1</v>
+      </c>
+      <c r="T10">
+        <v>1</v>
+      </c>
+      <c r="U10">
+        <v>1</v>
+      </c>
+      <c r="V10">
+        <v>1</v>
+      </c>
+      <c r="W10">
+        <v>1</v>
+      </c>
+      <c r="X10">
+        <v>1</v>
+      </c>
+      <c r="Y10">
+        <v>1</v>
+      </c>
+      <c r="Z10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+      <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="Q11">
+        <v>1</v>
+      </c>
+      <c r="R11">
+        <v>1</v>
+      </c>
+      <c r="S11">
+        <v>1</v>
+      </c>
+      <c r="T11">
+        <v>1</v>
+      </c>
+      <c r="U11">
+        <v>1</v>
+      </c>
+      <c r="V11">
+        <v>1</v>
+      </c>
+      <c r="W11">
+        <v>1</v>
+      </c>
+      <c r="X11">
+        <v>1</v>
+      </c>
+      <c r="Y11">
+        <v>1</v>
+      </c>
+      <c r="Z11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="Q12">
+        <v>1</v>
+      </c>
+      <c r="R12">
+        <v>1</v>
+      </c>
+      <c r="S12">
+        <v>1</v>
+      </c>
+      <c r="T12">
+        <v>1</v>
+      </c>
+      <c r="U12">
+        <v>1</v>
+      </c>
+      <c r="V12">
+        <v>1</v>
+      </c>
+      <c r="W12">
+        <v>1</v>
+      </c>
+      <c r="X12">
+        <v>1</v>
+      </c>
+      <c r="Y12">
+        <v>1</v>
+      </c>
+      <c r="Z12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+      <c r="O13">
+        <v>1</v>
+      </c>
+      <c r="P13">
+        <v>1</v>
+      </c>
+      <c r="Q13">
+        <v>1</v>
+      </c>
+      <c r="R13">
+        <v>1</v>
+      </c>
+      <c r="S13">
+        <v>1</v>
+      </c>
+      <c r="T13">
+        <v>1</v>
+      </c>
+      <c r="U13">
+        <v>1</v>
+      </c>
+      <c r="V13">
+        <v>1</v>
+      </c>
+      <c r="W13">
+        <v>1</v>
+      </c>
+      <c r="X13">
+        <v>1</v>
+      </c>
+      <c r="Y13">
+        <v>1</v>
+      </c>
+      <c r="Z13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="O14">
+        <v>1</v>
+      </c>
+      <c r="P14">
+        <v>1</v>
+      </c>
+      <c r="Q14">
+        <v>1</v>
+      </c>
+      <c r="R14" s="4">
+        <v>2</v>
+      </c>
+      <c r="S14" s="4">
+        <v>2</v>
+      </c>
+      <c r="T14">
+        <v>1</v>
+      </c>
+      <c r="U14">
+        <v>1</v>
+      </c>
+      <c r="V14">
+        <v>1</v>
+      </c>
+      <c r="W14">
+        <v>1</v>
+      </c>
+      <c r="X14">
+        <v>1</v>
+      </c>
+      <c r="Y14">
+        <v>1</v>
+      </c>
+      <c r="Z14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
+      <c r="O15">
+        <v>1</v>
+      </c>
+      <c r="P15">
+        <v>1</v>
+      </c>
+      <c r="Q15">
+        <v>1</v>
+      </c>
+      <c r="R15">
+        <v>1</v>
+      </c>
+      <c r="S15">
+        <v>1</v>
+      </c>
+      <c r="T15">
+        <v>1</v>
+      </c>
+      <c r="U15">
+        <v>1</v>
+      </c>
+      <c r="V15">
+        <v>1</v>
+      </c>
+      <c r="W15">
+        <v>1</v>
+      </c>
+      <c r="X15">
+        <v>1</v>
+      </c>
+      <c r="Y15">
+        <v>1</v>
+      </c>
+      <c r="Z15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <v>1</v>
+      </c>
+      <c r="N16">
+        <v>1</v>
+      </c>
+      <c r="O16">
+        <v>1</v>
+      </c>
+      <c r="P16">
+        <v>1</v>
+      </c>
+      <c r="Q16">
+        <v>1</v>
+      </c>
+      <c r="R16">
+        <v>1</v>
+      </c>
+      <c r="S16">
+        <v>1</v>
+      </c>
+      <c r="T16">
+        <v>1</v>
+      </c>
+      <c r="U16">
+        <v>1</v>
+      </c>
+      <c r="V16">
+        <v>1</v>
+      </c>
+      <c r="W16">
+        <v>1</v>
+      </c>
+      <c r="X16">
+        <v>1</v>
+      </c>
+      <c r="Y16">
+        <v>1</v>
+      </c>
+      <c r="Z16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <v>1</v>
+      </c>
+      <c r="M17">
+        <v>1</v>
+      </c>
+      <c r="N17">
+        <v>1</v>
+      </c>
+      <c r="O17">
+        <v>1</v>
+      </c>
+      <c r="P17">
+        <v>1</v>
+      </c>
+      <c r="Q17">
+        <v>1</v>
+      </c>
+      <c r="R17">
+        <v>1</v>
+      </c>
+      <c r="S17">
+        <v>1</v>
+      </c>
+      <c r="T17">
+        <v>1</v>
+      </c>
+      <c r="U17">
+        <v>1</v>
+      </c>
+      <c r="V17">
+        <v>1</v>
+      </c>
+      <c r="W17">
+        <v>1</v>
+      </c>
+      <c r="X17">
+        <v>1</v>
+      </c>
+      <c r="Y17">
+        <v>1</v>
+      </c>
+      <c r="Z17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <v>1</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
+      </c>
+      <c r="O18">
+        <v>1</v>
+      </c>
+      <c r="P18">
+        <v>1</v>
+      </c>
+      <c r="Q18">
+        <v>1</v>
+      </c>
+      <c r="R18">
+        <v>1</v>
+      </c>
+      <c r="S18">
+        <v>1</v>
+      </c>
+      <c r="T18">
+        <v>1</v>
+      </c>
+      <c r="U18">
+        <v>1</v>
+      </c>
+      <c r="V18">
+        <v>1</v>
+      </c>
+      <c r="W18">
+        <v>1</v>
+      </c>
+      <c r="X18">
+        <v>1</v>
+      </c>
+      <c r="Y18">
+        <v>1</v>
+      </c>
+      <c r="Z18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+      <c r="N19">
+        <v>1</v>
+      </c>
+      <c r="O19">
+        <v>1</v>
+      </c>
+      <c r="P19">
+        <v>1</v>
+      </c>
+      <c r="Q19">
+        <v>1</v>
+      </c>
+      <c r="R19">
+        <v>1</v>
+      </c>
+      <c r="S19">
+        <v>1</v>
+      </c>
+      <c r="T19">
+        <v>1</v>
+      </c>
+      <c r="U19">
+        <v>1</v>
+      </c>
+      <c r="V19">
+        <v>1</v>
+      </c>
+      <c r="W19">
+        <v>1</v>
+      </c>
+      <c r="X19">
+        <v>1</v>
+      </c>
+      <c r="Y19">
+        <v>1</v>
+      </c>
+      <c r="Z19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <v>1</v>
+      </c>
+      <c r="O20">
+        <v>1</v>
+      </c>
+      <c r="P20">
+        <v>1</v>
+      </c>
+      <c r="Q20">
+        <v>1</v>
+      </c>
+      <c r="R20">
+        <v>1</v>
+      </c>
+      <c r="S20">
+        <v>1</v>
+      </c>
+      <c r="T20">
+        <v>1</v>
+      </c>
+      <c r="U20">
+        <v>1</v>
+      </c>
+      <c r="V20">
+        <v>1</v>
+      </c>
+      <c r="W20">
+        <v>1</v>
+      </c>
+      <c r="X20">
+        <v>1</v>
+      </c>
+      <c r="Y20">
+        <v>1</v>
+      </c>
+      <c r="Z20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+      <c r="K21">
+        <v>1</v>
+      </c>
+      <c r="L21">
+        <v>1</v>
+      </c>
+      <c r="M21">
+        <v>1</v>
+      </c>
+      <c r="N21">
+        <v>1</v>
+      </c>
+      <c r="O21">
+        <v>1</v>
+      </c>
+      <c r="P21">
+        <v>1</v>
+      </c>
+      <c r="Q21">
+        <v>1</v>
+      </c>
+      <c r="R21">
+        <v>1</v>
+      </c>
+      <c r="S21">
+        <v>1</v>
+      </c>
+      <c r="T21">
+        <v>1</v>
+      </c>
+      <c r="U21">
+        <v>1</v>
+      </c>
+      <c r="V21">
+        <v>1</v>
+      </c>
+      <c r="W21">
+        <v>1</v>
+      </c>
+      <c r="X21">
+        <v>1</v>
+      </c>
+      <c r="Y21">
+        <v>1</v>
+      </c>
+      <c r="Z21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+      <c r="K22">
+        <v>1</v>
+      </c>
+      <c r="L22">
+        <v>1</v>
+      </c>
+      <c r="M22">
+        <v>1</v>
+      </c>
+      <c r="N22">
+        <v>1</v>
+      </c>
+      <c r="O22">
+        <v>1</v>
+      </c>
+      <c r="P22">
+        <v>1</v>
+      </c>
+      <c r="Q22">
+        <v>1</v>
+      </c>
+      <c r="R22">
+        <v>1</v>
+      </c>
+      <c r="S22">
+        <v>1</v>
+      </c>
+      <c r="T22">
+        <v>1</v>
+      </c>
+      <c r="U22">
+        <v>1</v>
+      </c>
+      <c r="V22">
+        <v>1</v>
+      </c>
+      <c r="W22">
+        <v>1</v>
+      </c>
+      <c r="X22">
+        <v>1</v>
+      </c>
+      <c r="Y22">
+        <v>1</v>
+      </c>
+      <c r="Z22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <v>1</v>
+      </c>
+      <c r="K23">
+        <v>1</v>
+      </c>
+      <c r="L23">
+        <v>1</v>
+      </c>
+      <c r="M23">
+        <v>1</v>
+      </c>
+      <c r="N23">
+        <v>1</v>
+      </c>
+      <c r="O23">
+        <v>1</v>
+      </c>
+      <c r="P23">
+        <v>1</v>
+      </c>
+      <c r="Q23">
+        <v>1</v>
+      </c>
+      <c r="R23">
+        <v>1</v>
+      </c>
+      <c r="S23">
+        <v>1</v>
+      </c>
+      <c r="T23">
+        <v>1</v>
+      </c>
+      <c r="U23">
+        <v>1</v>
+      </c>
+      <c r="V23">
+        <v>1</v>
+      </c>
+      <c r="W23">
+        <v>1</v>
+      </c>
+      <c r="X23">
+        <v>1</v>
+      </c>
+      <c r="Y23">
+        <v>1</v>
+      </c>
+      <c r="Z23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <v>1</v>
+      </c>
+      <c r="K24">
+        <v>1</v>
+      </c>
+      <c r="L24">
+        <v>1</v>
+      </c>
+      <c r="M24">
+        <v>1</v>
+      </c>
+      <c r="N24">
+        <v>1</v>
+      </c>
+      <c r="O24">
+        <v>1</v>
+      </c>
+      <c r="P24">
+        <v>1</v>
+      </c>
+      <c r="Q24">
+        <v>1</v>
+      </c>
+      <c r="R24">
+        <v>1</v>
+      </c>
+      <c r="S24">
+        <v>1</v>
+      </c>
+      <c r="T24">
+        <v>1</v>
+      </c>
+      <c r="U24">
+        <v>1</v>
+      </c>
+      <c r="V24">
+        <v>1</v>
+      </c>
+      <c r="W24">
+        <v>1</v>
+      </c>
+      <c r="X24">
+        <v>1</v>
+      </c>
+      <c r="Y24">
+        <v>1</v>
+      </c>
+      <c r="Z24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>1</v>
+      </c>
+      <c r="J25">
+        <v>1</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+      <c r="L25">
+        <v>1</v>
+      </c>
+      <c r="M25">
+        <v>1</v>
+      </c>
+      <c r="N25">
+        <v>1</v>
+      </c>
+      <c r="O25">
+        <v>1</v>
+      </c>
+      <c r="P25">
+        <v>1</v>
+      </c>
+      <c r="Q25">
+        <v>1</v>
+      </c>
+      <c r="R25">
+        <v>1</v>
+      </c>
+      <c r="S25">
+        <v>1</v>
+      </c>
+      <c r="T25">
+        <v>1</v>
+      </c>
+      <c r="U25">
+        <v>1</v>
+      </c>
+      <c r="V25">
+        <v>1</v>
+      </c>
+      <c r="W25">
+        <v>1</v>
+      </c>
+      <c r="X25">
+        <v>1</v>
+      </c>
+      <c r="Y25">
+        <v>1</v>
+      </c>
+      <c r="Z25">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>